<commit_message>
Parse txt and generate excel file done
</commit_message>
<xml_diff>
--- a/SPI.xlsx
+++ b/SPI.xlsx
@@ -820,7 +820,7 @@
   <dimension ref="A2:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -886,7 +886,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>